<commit_message>
update package init code
</commit_message>
<xml_diff>
--- a/Assets/data.xlsx
+++ b/Assets/data.xlsx
@@ -431,49 +431,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>主力流入1054亿</t>
+          <t>主力流入1408亿</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>主力流出1046亿</t>
+          <t>主力流出1514亿</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>主力净流入7.636亿</t>
+          <t>主力净流入-106.2亿</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>超大单347.2亿326.8亿</t>
+          <t>超大单462.8亿525.6亿</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>大单706.6亿719.4亿</t>
+          <t>大单945.2亿988.5亿</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>中单1062亿1092亿</t>
+          <t>中单1350亿1344亿</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>小单1092亿1069亿</t>
+          <t>小单1293亿1193亿</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update process thread code
</commit_message>
<xml_diff>
--- a/Assets/data.xlsx
+++ b/Assets/data.xlsx
@@ -431,49 +431,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>主力流入1408亿</t>
+          <t>主力流入1286亿</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>主力流出1514亿</t>
+          <t>主力流出1421亿</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>主力净流入-106.2亿</t>
+          <t>主力净流入-134.8亿</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>超大单462.8亿525.6亿</t>
+          <t>超大单418.6亿491.1亿</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>大单945.2亿988.5亿</t>
+          <t>大单867.8亿930.0亿</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>中单1350亿1344亿</t>
+          <t>中单1259亿1227亿</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>小单1293亿1193亿</t>
+          <t>小单1247亿1144亿</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add python embed web pages
</commit_message>
<xml_diff>
--- a/Assets/data.xlsx
+++ b/Assets/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,55 +428,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>主力流入1120亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>主力流出1252亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>主力净流入-131.4亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>超大单370.9亿449.8亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>大单749.4亿801.9亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>中单1122亿1091亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>小单1145亿1045亿</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add crawler stock code
</commit_message>
<xml_diff>
--- a/Assets/data.xlsx
+++ b/Assets/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,55 +428,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>主力流入1048亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>主力流出1178亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>主力净流入-130.6亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>超大单316.9亿393.3亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>大单730.9亿785.1亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>中单1078亿1047亿</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>小单1085亿984.6亿</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>